<commit_message>
push new branch to seevision automation
</commit_message>
<xml_diff>
--- a/test_case/before_fota_data.xlsx
+++ b/test_case/before_fota_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CBE158-41AA-034F-8F83-8CC5C3BDD410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A0C5FF-9C82-404D-AC81-7E5D64614A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6090" yWindow="1365" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="before_fota" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -122,7 +122,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,16 +459,16 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="192" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.375" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +479,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -490,7 +490,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -501,7 +501,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -512,7 +512,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -523,7 +523,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -534,7 +534,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -545,7 +545,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -556,7 +556,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -567,7 +567,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -578,7 +578,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -589,7 +589,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -600,7 +600,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>